<commit_message>
Some refactoring to remove pitt-specific stuff and to make setup.py closed to pypa's guide...-
</commit_message>
<xml_diff>
--- a/pycounter/test/data/JR1.xlsx
+++ b/pycounter/test/data/JR1.xlsx
@@ -1,13 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <workbookPr date1904="false"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Techuser\Documents\pycounter\pycounter\test\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22680" windowHeight="9555"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet0" r:id="rId3" sheetId="1"/>
+    <sheet name="Sheet0" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -20,9 +27,6 @@
     <t>Number of Successful Full-Text Article Requests by Month and Journal</t>
   </si>
   <si>
-    <t>University of Pittsburgh</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
@@ -726,66 +730,50 @@
   </si>
   <si>
     <t>455</t>
+  </si>
+  <si>
+    <t>University of Maximegalon</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="8"/>
       <name val="Arial"/>
-      <sz val="10.0"/>
-      <color indexed="8"/>
-      <u val="none"/>
     </font>
     <font>
+      <sz val="9"/>
+      <color indexed="8"/>
       <name val="Arial"/>
-      <sz val="9.0"/>
-      <b val="true"/>
-      <color indexed="8"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="9.0"/>
-      <color indexed="8"/>
-      <u val="none"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="darkGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
-      <patternFill>
-        <fgColor rgb="578FAE"/>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF578FAE"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="578FAE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill>
-        <fgColor rgb="BCD2DE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="BCD2DE"/>
+        <fgColor rgb="FFBCD2DE"/>
       </patternFill>
     </fill>
   </fills>
@@ -803,59 +791,316 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true" applyNumberFormat="true">
-      <alignment horizontal="left" vertical="top" wrapText="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="true" applyNumberFormat="true" applyFill="true">
-      <alignment horizontal="left" vertical="bottom" wrapText="false"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="true" applyNumberFormat="true" applyFill="true">
-      <alignment horizontal="left" vertical="bottom" wrapText="true"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="true" applyNumberFormat="true" applyFill="true">
-      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="true" applyNumberFormat="true">
-      <alignment horizontal="left" vertical="top" wrapText="true"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:V20"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="true" showGridLines="true"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.9375" customWidth="true"/>
-    <col min="2" max="2" width="35.9375" customWidth="true"/>
-    <col min="3" max="3" width="10.78125" customWidth="true"/>
-    <col min="4" max="4" width="10.78125" customWidth="true"/>
-    <col min="5" max="5" width="10.78125" customWidth="true"/>
-    <col min="6" max="6" width="10.78125" customWidth="true"/>
-    <col min="7" max="7" width="10.78125" customWidth="true"/>
-    <col min="8" max="8" width="10.78125" customWidth="true"/>
-    <col min="9" max="9" width="10.78125" customWidth="true"/>
-    <col min="10" max="10" width="10.78125" customWidth="true"/>
-    <col min="11" max="11" width="5.390625" customWidth="true"/>
-    <col min="12" max="12" width="5.390625" customWidth="true"/>
-    <col min="13" max="13" width="5.390625" customWidth="true"/>
-    <col min="14" max="14" width="5.390625" customWidth="true"/>
-    <col min="15" max="15" width="5.390625" customWidth="true"/>
-    <col min="16" max="16" width="5.390625" customWidth="true"/>
-    <col min="17" max="17" width="5.390625" customWidth="true"/>
-    <col min="18" max="18" width="5.390625" customWidth="true"/>
-    <col min="19" max="19" width="5.390625" customWidth="true"/>
-    <col min="20" max="20" width="5.390625" customWidth="true"/>
-    <col min="21" max="21" width="5.390625" customWidth="true"/>
-    <col min="22" max="22" width="5.390625" customWidth="true"/>
-    <col min="23" max="23" width="213.828125" customWidth="true"/>
+    <col min="1" max="2" width="36" customWidth="1"/>
+    <col min="3" max="10" width="10.7109375" customWidth="1"/>
+    <col min="11" max="22" width="5.42578125" customWidth="1"/>
+    <col min="23" max="23" width="213.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="16.0" customHeight="true">
+    <row r="1" spans="1:22" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -863,867 +1108,867 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" ht="16.0" customHeight="true">
+    <row r="2" spans="1:22" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" ht="16.0" customHeight="true">
-      <c r="A3" s="1" t="s">
+    <row r="4" spans="1:22" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" ht="16.0" customHeight="true">
-      <c r="A4" s="1" t="s">
+    <row r="5" spans="1:22" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" ht="16.0" customHeight="true">
-      <c r="A5" s="1" t="s">
+    <row r="6" spans="1:22" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" ht="16.0" customHeight="true">
-      <c r="A6" s="1" t="s">
+    <row r="7" spans="1:22" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" ht="12.0" customHeight="true">
-      <c r="A7" s="1" t="s">
+    <row r="8" spans="1:22" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="B8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="M8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="N8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="P8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="R8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="S8" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="T8" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="U8" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="V8" s="3" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="8" ht="45.0" customHeight="true">
-      <c r="A8" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K8" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="L8" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="M8" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="N8" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="O8" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="P8" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q8" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="R8" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="S8" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="T8" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="U8" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="V8" s="3" t="s">
+    <row r="9" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>29</v>
-      </c>
-    </row>
-    <row r="9" ht="15.0" customHeight="true">
-      <c r="A9" s="4" t="s">
-        <v>30</v>
       </c>
       <c r="B9" s="4"/>
       <c r="C9" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
       <c r="H9" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="I9" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="I9" s="4" t="s">
+      <c r="J9" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="J9" s="4" t="s">
+      <c r="K9" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="K9" s="4" t="s">
+      <c r="L9" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="L9" s="4" t="s">
+      <c r="M9" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="M9" s="4" t="s">
+      <c r="N9" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="N9" s="4" t="s">
+      <c r="O9" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="O9" s="4" t="s">
+      <c r="P9" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="P9" s="4" t="s">
+      <c r="Q9" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="Q9" s="4" t="s">
+      <c r="R9" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="R9" s="4" t="s">
+      <c r="S9" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="S9" s="4" t="s">
+      <c r="T9" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="T9" s="4" t="s">
+      <c r="U9" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="U9" s="4" t="s">
+      <c r="V9" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="V9" s="4" t="s">
+    </row>
+    <row r="10" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="10" ht="15.0" customHeight="true">
-      <c r="A10" s="5" t="s">
+      <c r="B10" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>48</v>
-      </c>
       <c r="C10" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G10" s="5"/>
       <c r="H10" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="I10" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="I10" s="5" t="s">
+      <c r="J10" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="J10" s="5" t="s">
+      <c r="K10" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="K10" s="5" t="s">
+      <c r="L10" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="L10" s="5" t="s">
+      <c r="M10" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="M10" s="5" t="s">
+      <c r="N10" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="N10" s="5" t="s">
+      <c r="O10" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="O10" s="5" t="s">
+      <c r="P10" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="P10" s="5" t="s">
+      <c r="Q10" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="Q10" s="5" t="s">
+      <c r="R10" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="R10" s="5" t="s">
+      <c r="S10" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="S10" s="5" t="s">
+      <c r="T10" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="T10" s="5" t="s">
+      <c r="U10" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="U10" s="5" t="s">
+      <c r="V10" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="V10" s="5" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="11" ht="15.0" customHeight="true">
-      <c r="A11" s="5" t="s">
-        <v>64</v>
-      </c>
       <c r="B11" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
       <c r="F11" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="G11" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="G11" s="5" t="s">
+      <c r="H11" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="H11" s="5" t="s">
+      <c r="I11" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="I11" s="5" t="s">
+      <c r="J11" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="J11" s="5" t="s">
+      <c r="K11" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="K11" s="5" t="s">
+      <c r="L11" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="L11" s="5" t="s">
+      <c r="M11" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="M11" s="5" t="s">
+      <c r="N11" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="N11" s="5" t="s">
+      <c r="O11" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="O11" s="5" t="s">
+      <c r="P11" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="P11" s="5" t="s">
+      <c r="Q11" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="Q11" s="5" t="s">
+      <c r="R11" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="R11" s="5" t="s">
+      <c r="S11" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="S11" s="5" t="s">
+      <c r="T11" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="T11" s="5" t="s">
+      <c r="U11" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="U11" s="5" t="s">
+      <c r="V11" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="V11" s="5" t="s">
+    </row>
+    <row r="12" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="12" ht="15.0" customHeight="true">
-      <c r="A12" s="5" t="s">
-        <v>82</v>
-      </c>
       <c r="B12" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
       <c r="F12" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="G12" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="G12" s="5" t="s">
+      <c r="H12" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="H12" s="5" t="s">
+      <c r="I12" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="I12" s="5" t="s">
+      <c r="J12" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="J12" s="5" t="s">
+      <c r="K12" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="K12" s="5" t="s">
+      <c r="L12" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="L12" s="5" t="s">
+      <c r="M12" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="M12" s="5" t="s">
+      <c r="N12" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="N12" s="5" t="s">
+      <c r="O12" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="O12" s="5" t="s">
+      <c r="P12" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="P12" s="5" t="s">
+      <c r="Q12" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="Q12" s="5" t="s">
+      <c r="R12" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="R12" s="5" t="s">
+      <c r="S12" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="S12" s="5" t="s">
+      <c r="T12" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="T12" s="5" t="s">
+      <c r="U12" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="U12" s="5" t="s">
+      <c r="V12" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="V12" s="5" t="s">
+    </row>
+    <row r="13" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="13" ht="15.0" customHeight="true">
-      <c r="A13" s="5" t="s">
-        <v>100</v>
-      </c>
       <c r="B13" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
       <c r="F13" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="G13" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="G13" s="5" t="s">
+      <c r="H13" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="H13" s="5" t="s">
+      <c r="I13" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="I13" s="5" t="s">
+      <c r="J13" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="J13" s="5" t="s">
+      <c r="K13" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="K13" s="5" t="s">
+      <c r="L13" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="L13" s="5" t="s">
+      <c r="M13" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="M13" s="5" t="s">
+      <c r="N13" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="N13" s="5" t="s">
+      <c r="O13" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="O13" s="5" t="s">
+      <c r="P13" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="P13" s="5" t="s">
+      <c r="Q13" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="Q13" s="5" t="s">
+      <c r="R13" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="R13" s="5" t="s">
+      <c r="S13" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="T13" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="S13" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="T13" s="5" t="s">
+      <c r="U13" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="U13" s="5" t="s">
+      <c r="V13" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="V13" s="5" t="s">
+    </row>
+    <row r="14" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="14" ht="15.0" customHeight="true">
-      <c r="A14" s="5" t="s">
-        <v>117</v>
-      </c>
       <c r="B14" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="G14" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="G14" s="5" t="s">
+      <c r="H14" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="H14" s="5" t="s">
+      <c r="I14" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="I14" s="5" t="s">
+      <c r="J14" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="J14" s="5" t="s">
+      <c r="K14" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="K14" s="5" t="s">
+      <c r="L14" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="L14" s="5" t="s">
+      <c r="M14" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="M14" s="5" t="s">
+      <c r="N14" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="N14" s="5" t="s">
+      <c r="O14" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="O14" s="5" t="s">
+      <c r="P14" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="P14" s="5" t="s">
+      <c r="Q14" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="Q14" s="5" t="s">
+      <c r="R14" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="R14" s="5" t="s">
+      <c r="S14" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="S14" s="5" t="s">
+      <c r="T14" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="T14" s="5" t="s">
+      <c r="U14" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="U14" s="5" t="s">
+      <c r="V14" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="V14" s="5" t="s">
+    </row>
+    <row r="15" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="15" ht="15.0" customHeight="true">
-      <c r="A15" s="5" t="s">
-        <v>135</v>
-      </c>
       <c r="B15" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
       <c r="F15" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="G15" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="G15" s="5" t="s">
+      <c r="H15" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="H15" s="5" t="s">
+      <c r="I15" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="I15" s="5" t="s">
+      <c r="J15" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="J15" s="5" t="s">
+      <c r="K15" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="K15" s="5" t="s">
+      <c r="L15" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="L15" s="5" t="s">
+      <c r="M15" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="M15" s="5" t="s">
+      <c r="N15" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="N15" s="5" t="s">
+      <c r="O15" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="O15" s="5" t="s">
+      <c r="P15" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="P15" s="5" t="s">
+      <c r="Q15" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="Q15" s="5" t="s">
+      <c r="R15" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="R15" s="5" t="s">
+      <c r="S15" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="S15" s="5" t="s">
+      <c r="T15" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="T15" s="5" t="s">
+      <c r="U15" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="U15" s="5" t="s">
+      <c r="V15" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="V15" s="5" t="s">
+    </row>
+    <row r="16" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="16" ht="15.0" customHeight="true">
-      <c r="A16" s="5" t="s">
-        <v>153</v>
-      </c>
       <c r="B16" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
       <c r="F16" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="G16" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="G16" s="5" t="s">
+      <c r="H16" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="H16" s="5" t="s">
+      <c r="I16" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="I16" s="5" t="s">
+      <c r="J16" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="J16" s="5" t="s">
+      <c r="K16" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="K16" s="5" t="s">
+      <c r="L16" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="L16" s="5" t="s">
+      <c r="M16" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="M16" s="5" t="s">
+      <c r="N16" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="N16" s="5" t="s">
+      <c r="O16" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="O16" s="5" t="s">
+      <c r="P16" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="P16" s="5" t="s">
+      <c r="Q16" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="Q16" s="5" t="s">
+      <c r="R16" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="R16" s="5" t="s">
+      <c r="S16" s="5" t="s">
         <v>166</v>
       </c>
-      <c r="S16" s="5" t="s">
+      <c r="T16" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="T16" s="5" t="s">
+      <c r="U16" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="U16" s="5" t="s">
+      <c r="V16" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="V16" s="5" t="s">
+    </row>
+    <row r="17" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="17" ht="15.0" customHeight="true">
-      <c r="A17" s="5" t="s">
-        <v>171</v>
-      </c>
       <c r="B17" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
       <c r="F17" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="G17" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="G17" s="5" t="s">
+      <c r="H17" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="H17" s="5" t="s">
+      <c r="I17" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="I17" s="5" t="s">
+      <c r="J17" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="J17" s="5" t="s">
+      <c r="K17" s="5" t="s">
         <v>176</v>
       </c>
-      <c r="K17" s="5" t="s">
+      <c r="L17" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="L17" s="5" t="s">
+      <c r="M17" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="M17" s="5" t="s">
+      <c r="N17" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="N17" s="5" t="s">
+      <c r="O17" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="P17" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="O17" s="5" t="s">
+      <c r="Q17" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="R17" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="S17" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="T17" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="U17" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="V17" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="P17" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="Q17" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="R17" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="S17" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="T17" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="U17" s="5" t="s">
+    </row>
+    <row r="18" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="V17" s="5" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="18" ht="15.0" customHeight="true">
-      <c r="A18" s="5" t="s">
-        <v>187</v>
-      </c>
       <c r="B18" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
       <c r="F18" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="G18" s="5" t="s">
         <v>188</v>
       </c>
-      <c r="G18" s="5" t="s">
+      <c r="H18" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="H18" s="5" t="s">
+      <c r="I18" s="5" t="s">
         <v>190</v>
       </c>
-      <c r="I18" s="5" t="s">
+      <c r="J18" s="5" t="s">
         <v>191</v>
       </c>
-      <c r="J18" s="5" t="s">
+      <c r="K18" s="5" t="s">
         <v>192</v>
       </c>
-      <c r="K18" s="5" t="s">
+      <c r="L18" s="5" t="s">
         <v>193</v>
       </c>
-      <c r="L18" s="5" t="s">
+      <c r="M18" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="M18" s="5" t="s">
+      <c r="N18" s="5" t="s">
         <v>195</v>
       </c>
-      <c r="N18" s="5" t="s">
+      <c r="O18" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="O18" s="5" t="s">
+      <c r="P18" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="P18" s="5" t="s">
+      <c r="Q18" s="5" t="s">
         <v>198</v>
       </c>
-      <c r="Q18" s="5" t="s">
+      <c r="R18" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="R18" s="5" t="s">
+      <c r="S18" s="5" t="s">
         <v>200</v>
       </c>
-      <c r="S18" s="5" t="s">
+      <c r="T18" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="T18" s="5" t="s">
+      <c r="U18" s="5" t="s">
         <v>202</v>
       </c>
-      <c r="U18" s="5" t="s">
+      <c r="V18" s="5" t="s">
         <v>203</v>
       </c>
-      <c r="V18" s="5" t="s">
+    </row>
+    <row r="19" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="19" ht="15.0" customHeight="true">
-      <c r="A19" s="5" t="s">
-        <v>205</v>
-      </c>
       <c r="B19" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
       <c r="F19" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="G19" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="G19" s="5" t="s">
+      <c r="H19" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="H19" s="5" t="s">
+      <c r="I19" s="5" t="s">
         <v>208</v>
       </c>
-      <c r="I19" s="5" t="s">
+      <c r="J19" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="J19" s="5" t="s">
+      <c r="K19" s="5" t="s">
         <v>210</v>
       </c>
-      <c r="K19" s="5" t="s">
+      <c r="L19" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="L19" s="5" t="s">
+      <c r="M19" s="5" t="s">
         <v>212</v>
       </c>
-      <c r="M19" s="5" t="s">
+      <c r="N19" s="5" t="s">
         <v>213</v>
       </c>
-      <c r="N19" s="5" t="s">
+      <c r="O19" s="5" t="s">
         <v>214</v>
       </c>
-      <c r="O19" s="5" t="s">
+      <c r="P19" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="P19" s="5" t="s">
+      <c r="Q19" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="Q19" s="5" t="s">
+      <c r="R19" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="R19" s="5" t="s">
+      <c r="S19" s="5" t="s">
         <v>218</v>
       </c>
-      <c r="S19" s="5" t="s">
+      <c r="T19" s="5" t="s">
         <v>219</v>
       </c>
-      <c r="T19" s="5" t="s">
+      <c r="U19" s="5" t="s">
         <v>220</v>
       </c>
-      <c r="U19" s="5" t="s">
+      <c r="V19" s="5" t="s">
         <v>221</v>
       </c>
-      <c r="V19" s="5" t="s">
+    </row>
+    <row r="20" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="20" ht="15.0" customHeight="true">
-      <c r="A20" s="5" t="s">
-        <v>223</v>
-      </c>
       <c r="B20" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
       <c r="F20" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="G20" s="5" t="s">
         <v>224</v>
       </c>
-      <c r="G20" s="5" t="s">
+      <c r="H20" s="5" t="s">
         <v>225</v>
       </c>
-      <c r="H20" s="5" t="s">
+      <c r="I20" s="5" t="s">
         <v>226</v>
       </c>
-      <c r="I20" s="5" t="s">
+      <c r="J20" s="5" t="s">
         <v>227</v>
       </c>
-      <c r="J20" s="5" t="s">
+      <c r="K20" s="5" t="s">
         <v>228</v>
       </c>
-      <c r="K20" s="5" t="s">
+      <c r="L20" s="5" t="s">
         <v>229</v>
       </c>
-      <c r="L20" s="5" t="s">
+      <c r="M20" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="N20" s="5" t="s">
         <v>230</v>
       </c>
-      <c r="M20" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="N20" s="5" t="s">
+      <c r="O20" s="5" t="s">
         <v>231</v>
       </c>
-      <c r="O20" s="5" t="s">
+      <c r="P20" s="5" t="s">
         <v>232</v>
       </c>
-      <c r="P20" s="5" t="s">
+      <c r="Q20" s="5" t="s">
         <v>233</v>
       </c>
-      <c r="Q20" s="5" t="s">
+      <c r="R20" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="S20" s="5" t="s">
         <v>234</v>
       </c>
-      <c r="R20" s="5" t="s">
-        <v>167</v>
-      </c>
-      <c r="S20" s="5" t="s">
+      <c r="T20" s="5" t="s">
         <v>235</v>
       </c>
-      <c r="T20" s="5" t="s">
+      <c r="U20" s="5" t="s">
         <v>236</v>
       </c>
-      <c r="U20" s="5" t="s">
-        <v>237</v>
-      </c>
       <c r="V20" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
-  <printOptions gridLines="true"/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="landscape" scale="100" blackAndWhite="false" useFirstPageNumber="true" draft="false"/>
+  <printOptions gridLines="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" useFirstPageNumber="1"/>
 </worksheet>
 </file>
</xml_diff>